<commit_message>
Add change log and roadmap
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_Tipi_di_mutazione.xlsx
+++ b/src/_static/xlsx/tab_Tipi_di_mutazione.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="20115" windowHeight="5700"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19440" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Codice</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Completamento</t>
+  </si>
+  <si>
+    <t>Dati integrativi AIRE</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,6 +636,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -664,15 +675,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0EB43895666D743BBE5EE80DE8AFF2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3898ec998cc85d3bcc261598fbbf3dc9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -786,6 +788,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -793,14 +804,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EADACEF-51D5-4A38-9CE7-2DDFA85BD7D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A838EA3F-6D46-400D-B10E-D3AC744F50C3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -816,17 +819,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EADACEF-51D5-4A38-9CE7-2DDFA85BD7D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A83983-DAA3-4CE3-9477-78D8A0CBB621}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>